<commit_message>
Adding senderinfo on request and changing some mapping to helthcare-personal
</commit_message>
<xml_diff>
--- a/ServiceInteractions/local/druglist/docs/Mappningspecifikation-VAS.xlsx
+++ b/ServiceInteractions/local/druglist/docs/Mappningspecifikation-VAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="160" windowWidth="26460" windowHeight="14460" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28640" windowHeight="16580" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revisioner" sheetId="1" r:id="rId1"/>
@@ -21,16 +21,262 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
+  <si>
+    <t>GetSubjectOfCareDrugListType.SenderInfoType.sending_system</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListType.SenderInfoType.sending_user</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.CareUnitIdType.name_internal_clinic</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.CareUnitIdType.name_internal_establishment</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.CareUnitIdType.name_external_clinic</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>recept/klinkod</t>
+  </si>
+  <si>
+    <t>recept/inrkod</t>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.bats</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>VAS fält</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ordination/ordlopnr, recept/ordlopnr</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ordination/idnr, recept/idnr</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>recept/lpnr</t>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.DrugPrescriptionIdType.subject_of_care_application_id</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListType.SubjectOfCareIdType</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListType.DrugPrescriptionEnum</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListType.KnowPrescriptionType.ordination_serial_no</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListType.KnowPrescriptionType.drug_prescription_serial_no</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.ResultCodeEnum</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.comment</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResultCodeEnum.OK</t>
+  </si>
+  <si>
+    <t>ResultCodeEnum.Error</t>
+  </si>
+  <si>
+    <t>ResultCodeEnum.Info</t>
+  </si>
+  <si>
+    <t>Koder för resultat</t>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListType</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Ansvarig</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>Revisioner</t>
+  </si>
+  <si>
+    <t>Struktur</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>Mappning Response</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>Mats Ekhammar</t>
+  </si>
+  <si>
+    <t>Upprättad</t>
+  </si>
+  <si>
+    <t>^[0-9]{6}[0-9pPtTfF][0-9]{3}$</t>
+  </si>
+  <si>
+    <t>Constant for retrieving ALL or CURRENT</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALL, CURRENT</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rules/Patterns</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mappning Request</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>VAS Field</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Structure</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>recept.vgivkod</t>
+  </si>
+  <si>
+    <t>recept.regvgiv</t>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.name_responsible_health_care_personnel</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.atc_code</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.name_registering_carer</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.signing_date</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.registration_date</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.registration_time</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.execution_start_date</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.execution_end_date</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.dosage_code</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.dosage_type</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.drug_name</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.prescription_text</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.responsible_health_care_personnel</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.strength</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.strength_unit</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.strength_text</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.secrecy</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.treatment_time_days</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.quantity</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.DrugPrescriptionIdType.ordination_serial_no</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.DrugPrescriptionIdType.drug_prescription_serial_no</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.CareUnitIdType.clinic_code</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.CareUnitIdType.institution_code</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
   <si>
     <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.code_registering_carer</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>recept.vgivkod</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>recept.dosvardenh</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -94,9 +340,6 @@
     <t>recept/rectxt</t>
   </si>
   <si>
-    <t>recept/sign</t>
-  </si>
-  <si>
     <t>recept/strnum</t>
   </si>
   <si>
@@ -176,243 +419,7 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.name_signing_carer</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.name_of_substance</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.atc_code</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.name_registering_carer</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.signing_date</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.registration_date</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.registration_time</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.execution_start_date</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.execution_end_date</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.dosage_code</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.dosage_type</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.drug_name</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.prescription_text</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.responsible_health_care_personnel</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.strength</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.strength_unit</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.strength_text</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.secrecy</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.treatment_time_days</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.quantity</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.DrugPrescriptionIdType.ordination_serial_no</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.DrugPrescriptionIdType.drug_prescription_serial_no</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.CareUnitIdType.clinic_code</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.CareUnitIdType.institution_code</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.CareUnitIdType.name_internal_clinic</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.CareUnitIdType.name_internal_establishment</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.CareUnitIdType.name_external_clinic</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>recept/klinkod</t>
-  </si>
-  <si>
-    <t>recept/inrkod</t>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.bats</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>VAS fält</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ordination/ordlopnr, recept/ordlopnr</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ordination/idnr, recept/idnr</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>recept/lpnr</t>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.DrugPrescriptionType.DrugPrescriptionIdType.subject_of_care_application_id</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListType.SubjectOfCareIdType</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListType.DrugPrescriptionEnum</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListType.KnowPrescriptionType.ordination_serial_no</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListType.KnowPrescriptionType.drug_prescription_serial_no</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.ResultCodeEnum</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListResponseType.comment</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ResultCodeEnum.OK</t>
-  </si>
-  <si>
-    <t>ResultCodeEnum.Error</t>
-  </si>
-  <si>
-    <t>ResultCodeEnum.Info</t>
-  </si>
-  <si>
-    <t>Koder för resultat</t>
-  </si>
-  <si>
-    <t>GetSubjectOfCareDrugListType</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Datum</t>
-  </si>
-  <si>
-    <t>Ansvarig</t>
-  </si>
-  <si>
-    <t>Kommentar</t>
-  </si>
-  <si>
-    <t>Revisioner</t>
-  </si>
-  <si>
-    <t>Struktur</t>
-  </si>
-  <si>
-    <t>In</t>
-  </si>
-  <si>
-    <t>Mappning Response</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>Mats Ekhammar</t>
-  </si>
-  <si>
-    <t>Upprättad</t>
-  </si>
-  <si>
-    <t>^[0-9]{6}[0-9pPtTfF][0-9]{3}$</t>
-  </si>
-  <si>
-    <t>Constant for retrieving ALL or CURRENT</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALL, CURRENT</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rules/Patterns</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mappning Request</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>VAS Field</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Comment</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Structure</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -479,7 +486,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -687,21 +694,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -727,21 +719,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -829,34 +806,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1188,39 +1165,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21">
-      <c r="A1" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="A1" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1">
       <c r="A2" s="1" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickTop="1">
       <c r="A3" s="5" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="B3" s="6">
         <v>40235</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1386,6 +1363,7 @@
       <c r="D30" s="12"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -1423,10 +1401,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C1" activeCellId="1" sqref="A4:D5 A1:C1048576"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1438,7 +1416,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="15" customFormat="1" ht="26">
       <c r="A1" s="22" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="B1" s="22"/>
     </row>
@@ -1446,30 +1424,30 @@
       <c r="A3" s="25"/>
     </row>
     <row r="4" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42" t="s">
-        <v>105</v>
+      <c r="A4" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="44" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="17" customFormat="1" ht="15" thickBot="1">
       <c r="A5" s="29" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="43"/>
+        <v>41</v>
+      </c>
+      <c r="D5" s="45"/>
     </row>
     <row r="6" spans="1:4" s="17" customFormat="1">
       <c r="A6" s="24" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="30"/>
@@ -1477,54 +1455,70 @@
     </row>
     <row r="7" spans="1:4" s="17" customFormat="1">
       <c r="A7" s="18" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="32"/>
       <c r="D7" s="31" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="18" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="19" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="44" t="s">
-        <v>82</v>
+      <c r="A9" s="39" t="s">
+        <v>15</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
     </row>
-    <row r="10" spans="1:4" s="17" customFormat="1">
-      <c r="A10" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
+    <row r="10" spans="1:4">
+      <c r="A10" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-    </row>
-    <row r="13" spans="1:4" ht="16"/>
+      <c r="A11" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+    </row>
+    <row r="12" spans="1:4" s="17" customFormat="1">
+      <c r="A12" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:D5"/>
@@ -1542,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1558,7 +1552,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="15" customFormat="1" ht="26">
       <c r="A1" s="22" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="B1" s="22"/>
     </row>
@@ -1566,28 +1560,28 @@
       <c r="A2" s="25"/>
     </row>
     <row r="3" spans="1:5" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42" t="s">
-        <v>5</v>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="44" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="17" customFormat="1" ht="15" thickBot="1">
       <c r="A4" s="29" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="43"/>
+        <v>71</v>
+      </c>
+      <c r="D4" s="45"/>
     </row>
     <row r="5" spans="1:5" s="27" customFormat="1">
       <c r="A5" s="23" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="C5" s="26"/>
       <c r="D5" s="37"/>
@@ -1595,7 +1589,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="23" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="B6" s="36"/>
       <c r="C6" s="26"/>
@@ -1604,21 +1598,21 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="23" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="B7" s="36"/>
       <c r="C7" s="26"/>
       <c r="D7" s="31" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="23" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
@@ -1626,10 +1620,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
@@ -1637,10 +1631,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
@@ -1648,10 +1642,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
@@ -1659,10 +1653,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
@@ -1670,7 +1664,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="23" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="B13" s="36"/>
       <c r="C13" s="26"/>
@@ -1679,7 +1673,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="23" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="B14" s="36"/>
       <c r="C14" s="26"/>
@@ -1688,7 +1682,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="23" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="B15" s="36"/>
       <c r="C15" s="26"/>
@@ -1697,10 +1691,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="23" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
@@ -1708,10 +1702,10 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
@@ -1719,10 +1713,10 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
@@ -1730,10 +1724,10 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
@@ -1741,10 +1735,10 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
@@ -1752,10 +1746,10 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
@@ -1763,10 +1757,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
@@ -1774,10 +1768,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
@@ -1785,10 +1779,10 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
@@ -1796,10 +1790,10 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
@@ -1807,10 +1801,10 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
@@ -1818,10 +1812,10 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
@@ -1829,10 +1823,10 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="23" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
@@ -1840,10 +1834,10 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="23" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
@@ -1851,10 +1845,10 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="23" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
@@ -1871,7 +1865,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="23" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="B32" s="36"/>
       <c r="C32" s="26"/>
@@ -1880,10 +1874,10 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
@@ -1891,7 +1885,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="36"/>
       <c r="C34" s="26"/>
@@ -1900,10 +1894,10 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
@@ -1911,10 +1905,10 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
@@ -1922,10 +1916,10 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
@@ -1933,10 +1927,10 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
@@ -1944,10 +1938,10 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
@@ -1955,10 +1949,10 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="23" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
@@ -1966,10 +1960,10 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="23" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="C41" s="26"/>
       <c r="D41" s="26"/>
@@ -1977,10 +1971,10 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="23" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
@@ -1988,10 +1982,10 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="23" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -1999,86 +1993,82 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="23" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="23" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="23" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="C46" s="26"/>
       <c r="D46" s="26"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="23" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="C47" s="26"/>
       <c r="D47" s="26"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="23" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C48" s="26"/>
       <c r="D48" s="26"/>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="35" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="16"/>
-    <row r="58" spans="1:1" ht="16"/>
-    <row r="59" spans="1:1" ht="16"/>
-    <row r="60" spans="1:1" ht="16"/>
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:D4"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>